<commit_message>
Populated spreadsheet with results
</commit_message>
<xml_diff>
--- a/data_collection.xlsx
+++ b/data_collection.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
   <si>
     <t>User</t>
   </si>
@@ -58,13 +58,148 @@
   </si>
   <si>
     <t>How deal with stress?</t>
+  </si>
+  <si>
+    <t>Anything confusing?</t>
+  </si>
+  <si>
+    <t>Additional comments? (Like/dislike)</t>
+  </si>
+  <si>
+    <t>102/61</t>
+  </si>
+  <si>
+    <t>99/65</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Listen to music</t>
+  </si>
+  <si>
+    <t>Isn't relaxing to move head around - the butterflies move around too much. Made participant dizzy.</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>100/68</t>
+  </si>
+  <si>
+    <t>125/76</t>
+  </si>
+  <si>
+    <t>Hard to tell depth perception; difficult to see difference in depth. The white dot cursor is distracting (it moves when the head moves). Confused about whether the white dot is head or not.</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>128/79</t>
+  </si>
+  <si>
+    <t>Should add a calming scent on the nose bands to *really* make this relaxing.</t>
+  </si>
+  <si>
+    <t>Yoga when time but very infrequent; talking to friends</t>
+  </si>
+  <si>
+    <t>139/83</t>
+  </si>
+  <si>
+    <t>106/70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Butterflies moved too quicky; hard to feel connection between finger and blue dot. </t>
+  </si>
+  <si>
+    <t>Talking to friends on gChat, listening to music.</t>
+  </si>
+  <si>
+    <t>109/67</t>
+  </si>
+  <si>
+    <t>Would be cool to add breathing element.</t>
+  </si>
+  <si>
+    <t>124/93</t>
+  </si>
+  <si>
+    <t>116/80</t>
+  </si>
+  <si>
+    <t>114/79</t>
+  </si>
+  <si>
+    <t>Non-work-related stuff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3d space vs 2d space. </t>
+  </si>
+  <si>
+    <t>Initial prompt for how to move head around.</t>
+  </si>
+  <si>
+    <t>118/80</t>
+  </si>
+  <si>
+    <t>108/74</t>
+  </si>
+  <si>
+    <t>97/66</t>
+  </si>
+  <si>
+    <t>Does meditation normally.</t>
+  </si>
+  <si>
+    <t>Took a lot of time to understand what's going on. Sometimes it can be hard to see the butterflies because of the transparent screen. This only works if we face a wall.</t>
+  </si>
+  <si>
+    <t>Need to make sure butterflies are rendered in a good position.</t>
+  </si>
+  <si>
+    <t>106/68</t>
+  </si>
+  <si>
+    <t>102/71</t>
+  </si>
+  <si>
+    <t>Go on runs usually.</t>
+  </si>
+  <si>
+    <t>Hardest part was getting started; actually following butterflies was fine.</t>
+  </si>
+  <si>
+    <t>102/78</t>
+  </si>
+  <si>
+    <t>102/77</t>
+  </si>
+  <si>
+    <t>104/76</t>
+  </si>
+  <si>
+    <t>Exercise and breathing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Butterflies moved in an unintuitive way. </t>
+  </si>
+  <si>
+    <t>Bring it to the lab one more time!</t>
+  </si>
+  <si>
+    <t>110/60</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -76,6 +211,22 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,14 +249,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -435,15 +590,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
     <col min="5" max="6" width="28.6640625" customWidth="1"/>
@@ -452,10 +607,12 @@
     <col min="10" max="10" width="10.33203125" customWidth="1"/>
     <col min="11" max="11" width="19.6640625" customWidth="1"/>
     <col min="12" max="12" width="16.1640625" customWidth="1"/>
-    <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="13" max="13" width="24.6640625" customWidth="1"/>
+    <col min="14" max="14" width="84.1640625" customWidth="1"/>
+    <col min="15" max="15" width="66.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,109 +652,345 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2">
+        <v>61</v>
+      </c>
+      <c r="K2">
+        <v>69</v>
+      </c>
+      <c r="L2">
+        <v>62</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3">
+        <v>42</v>
+      </c>
+      <c r="K3">
+        <v>52</v>
+      </c>
+      <c r="L3">
+        <v>52</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4">
+        <v>75</v>
+      </c>
+      <c r="K4">
+        <v>75</v>
+      </c>
+      <c r="L4">
+        <v>49</v>
+      </c>
+      <c r="M4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5">
+        <v>62</v>
+      </c>
+      <c r="K5">
+        <v>68</v>
+      </c>
+      <c r="L5">
+        <v>65</v>
+      </c>
+      <c r="M5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6">
+        <v>71</v>
+      </c>
+      <c r="K6">
+        <v>71</v>
+      </c>
+      <c r="L6">
+        <v>73</v>
+      </c>
+      <c r="M6" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" t="s">
+        <v>45</v>
+      </c>
+      <c r="O6" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7">
+        <v>58</v>
+      </c>
+      <c r="K7">
+        <v>57</v>
+      </c>
+      <c r="L7">
+        <v>54</v>
+      </c>
+      <c r="M7" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" t="s">
+        <v>50</v>
+      </c>
+      <c r="O7" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21">
-        <v>20</v>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8">
+        <v>69</v>
+      </c>
+      <c r="K8">
+        <v>67</v>
+      </c>
+      <c r="L8">
+        <v>61</v>
+      </c>
+      <c r="M8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N8" t="s">
+        <v>55</v>
+      </c>
+      <c r="O8" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>